<commit_message>
data including monthly hydrogen
</commit_message>
<xml_diff>
--- a/data/competes_ENTSOE/monthly_H2_heat_demand.xlsx
+++ b/data/competes_ENTSOE/monthly_H2_heat_demand.xlsx
@@ -7,7 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="demand" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="prices" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -16,10 +17,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -58,12 +56,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -431,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,140 +447,356 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Industrial heat (fulfiled by electric boilers)</t>
+          <t>Industrial heat</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>total</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="n">
-        <v>43466</v>
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>2019-01-01_00:00:00</t>
+        </is>
       </c>
       <c r="B2" t="n">
-        <v>19586571.34720217</v>
+        <v>14494062.7969296</v>
       </c>
       <c r="C2" t="n">
-        <v>1192531.269469551</v>
+        <v>891387.0095024927</v>
+      </c>
+      <c r="D2" t="n">
+        <v>15385449.8064321</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="n">
-        <v>43496.41666666666</v>
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>2019-01-31_10:00:00</t>
+        </is>
       </c>
       <c r="B3" t="n">
-        <v>13631530.8526801</v>
+        <v>10087332.83098327</v>
       </c>
       <c r="C3" t="n">
-        <v>1750507.813883353</v>
+        <v>1308460.386135032</v>
+      </c>
+      <c r="D3" t="n">
+        <v>11395793.2171183</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="n">
-        <v>43526.83333333334</v>
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>2019-03-02_20:00:00</t>
+        </is>
       </c>
       <c r="B4" t="n">
-        <v>13631773.63838166</v>
+        <v>10087512.49240243</v>
       </c>
       <c r="C4" t="n">
-        <v>3985965.373592944</v>
+        <v>2979408.461069473</v>
+      </c>
+      <c r="D4" t="n">
+        <v>13066920.9534719</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="n">
-        <v>43557.25</v>
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>2019-04-02_06:00:00</t>
+        </is>
       </c>
       <c r="B5" t="n">
-        <v>9089903.047825094</v>
+        <v>6726528.25539057</v>
       </c>
       <c r="C5" t="n">
-        <v>4347171.679415486</v>
+        <v>3249401.053300465</v>
+      </c>
+      <c r="D5" t="n">
+        <v>9975929.308691034</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="n">
-        <v>43587.66666666666</v>
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>2019-05-02_16:00:00</t>
+        </is>
       </c>
       <c r="B6" t="n">
-        <v>15017606.06193918</v>
+        <v>11113028.48583499</v>
       </c>
       <c r="C6" t="n">
-        <v>4493368.979966091</v>
+        <v>3358679.843611017</v>
+      </c>
+      <c r="D6" t="n">
+        <v>14471708.32944601</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="2" t="n">
-        <v>43618.08333333334</v>
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>2019-06-02_02:00:00</t>
+        </is>
       </c>
       <c r="B7" t="n">
-        <v>12100940.93002706</v>
+        <v>8954696.288220024</v>
       </c>
       <c r="C7" t="n">
-        <v>4480976.734163946</v>
+        <v>3349416.952809414</v>
+      </c>
+      <c r="D7" t="n">
+        <v>12304113.24102944</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="2" t="n">
-        <v>43648.5</v>
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>2019-07-02_12:00:00</t>
+        </is>
       </c>
       <c r="B8" t="n">
-        <v>12915827.01573847</v>
+        <v>9557711.991646467</v>
       </c>
       <c r="C8" t="n">
-        <v>4469189.615826338</v>
+        <v>3340606.379506555</v>
+      </c>
+      <c r="D8" t="n">
+        <v>12898318.37115302</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="2" t="n">
-        <v>43678.91666666666</v>
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>2019-08-01_22:00:00</t>
+        </is>
       </c>
       <c r="B9" t="n">
-        <v>9874417.203945901</v>
+        <v>7307068.730919966</v>
       </c>
       <c r="C9" t="n">
-        <v>4489198.68953493</v>
+        <v>3355562.656824089</v>
+      </c>
+      <c r="D9" t="n">
+        <v>10662631.38774406</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="2" t="n">
-        <v>43709.33333333334</v>
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>2019-09-01_08:00:00</t>
+        </is>
       </c>
       <c r="B10" t="n">
-        <v>11306081.82232763</v>
+        <v>8366500.548522449</v>
       </c>
       <c r="C10" t="n">
-        <v>4493368.94958385</v>
+        <v>3358679.82090106</v>
+      </c>
+      <c r="D10" t="n">
+        <v>11725180.36942351</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="2" t="n">
-        <v>43739.75</v>
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>2019-10-01_18:00:00</t>
+        </is>
       </c>
       <c r="B11" t="n">
-        <v>5953973.090127265</v>
+        <v>4405940.086694176</v>
       </c>
       <c r="C11" t="n">
-        <v>4051990.5131052</v>
+        <v>3028760.585553382</v>
+      </c>
+      <c r="D11" t="n">
+        <v>7434700.672247559</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="2" t="n">
-        <v>43770.16666666666</v>
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>2019-11-01_04:00:00</t>
+        </is>
       </c>
       <c r="B12" t="n">
-        <v>18443564.21587624</v>
+        <v>13648237.51974842</v>
       </c>
       <c r="C12" t="n">
-        <v>4394827.486770224</v>
+        <v>3285022.565868652</v>
+      </c>
+      <c r="D12" t="n">
+        <v>16933260.08561707</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="2" t="n">
-        <v>43800.58333333334</v>
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>2019-12-01_14:00:00</t>
+        </is>
       </c>
       <c r="B13" t="n">
-        <v>20659687.09633049</v>
+        <v>15288168.45128457</v>
       </c>
       <c r="C13" t="n">
-        <v>4382563.894652126</v>
+        <v>3275855.840447044</v>
+      </c>
+      <c r="D13" t="n">
+        <v>18564024.29173161</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>hours</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>NED</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>2019-01-01_00:00:00</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>188.468197643773</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>2019-01-31_10:00:00</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>160.2863019909899</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>2019-03-02_20:00:00</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>110.7809744493958</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>2019-04-02_06:00:00</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>55.79715927674411</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>2019-05-02_16:00:00</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>55.4921684300246</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>2019-06-02_02:00:00</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>55.6175675413002</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>2019-07-02_12:00:00</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>55.5860344634459</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>2019-08-01_22:00:00</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>55.75963361921727</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>2019-09-01_08:00:00</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>63.5734283013198</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>2019-10-01_18:00:00</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>73.40910145377882</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>2019-11-01_04:00:00</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>70.42053777034438</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>2019-12-01_14:00:00</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>46.07482878091285</v>
       </c>
     </row>
   </sheetData>

</xml_diff>